<commit_message>
I don´t know. some safe before I mess it up
</commit_message>
<xml_diff>
--- a/Metadaten_all_86_cleanandneat.xlsx
+++ b/Metadaten_all_86_cleanandneat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="12850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="12852"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenf. Permafrost Data" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Zusammenf. Permafrost Data'!$B$16:$H$21</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="18">
   <si>
     <t>depth</t>
   </si>
@@ -75,6 +74,9 @@
   </si>
   <si>
     <t>Probe</t>
+  </si>
+  <si>
+    <t>weight</t>
   </si>
 </sst>
 </file>
@@ -522,26 +524,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O102"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="26.4140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="27" customWidth="1"/>
-    <col min="4" max="4" width="12.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.3984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.296875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.4140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3984375" style="1" customWidth="1"/>
     <col min="11" max="13" width="9" style="1"/>
     <col min="14" max="14" width="15.5" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -587,8 +589,11 @@
       <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -627,8 +632,11 @@
       <c r="O2" s="1">
         <v>2340</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -667,8 +675,11 @@
       <c r="O3" s="1">
         <v>2564.2718446601939</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -707,8 +718,11 @@
       <c r="O4" s="1">
         <v>3777.8640776699026</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -747,8 +761,11 @@
       <c r="O5" s="1">
         <v>8729.3203883495153</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -795,8 +812,11 @@
       <c r="O6" s="1">
         <v>16630</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -843,8 +863,11 @@
       <c r="O7" s="1">
         <v>16544.85436893204</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -891,8 +914,11 @@
       <c r="O8" s="1">
         <v>22056.369785794814</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -935,8 +961,11 @@
       <c r="O9" s="1">
         <v>23420.518602029311</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -983,8 +1012,11 @@
       <c r="O10" s="1">
         <v>26813.979706877115</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1031,8 +1063,11 @@
       <c r="O11" s="1">
         <v>29091.319052987601</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1079,8 +1114,11 @@
       <c r="O12" s="1">
         <v>34333.7091319053</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1121,8 +1159,11 @@
       <c r="O13" s="1">
         <v>36239.007891770008</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1163,8 +1204,11 @@
       <c r="O14" s="1">
         <v>40000</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1205,8 +1249,11 @@
       <c r="O15" s="1">
         <v>41639.233370913193</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P15" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1253,8 +1300,11 @@
       <c r="O16" s="1">
         <v>38000</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P16" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1302,8 +1352,11 @@
       <c r="O17" s="1">
         <v>38900.315000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P17" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1350,8 +1403,11 @@
       <c r="O18" s="1">
         <v>16915.631067961163</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P18" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1398,8 +1454,11 @@
       <c r="O19" s="1">
         <v>21770</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P19" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -1446,8 +1505,11 @@
       <c r="O20" s="1">
         <v>19342.815533980582</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P20" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1494,8 +1556,11 @@
       <c r="O21" s="1">
         <v>14488.446601941747</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1535,8 +1600,11 @@
       <c r="O22" s="1">
         <v>45.220700000000022</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1576,8 +1644,11 @@
       <c r="O23" s="1">
         <v>175</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1617,8 +1688,11 @@
       <c r="O24" s="1">
         <v>578.44395000000009</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -1658,8 +1732,11 @@
       <c r="O25" s="1">
         <v>956.86045000000013</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1706,8 +1783,11 @@
       <c r="O26" s="1">
         <v>1080</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1754,8 +1834,11 @@
       <c r="O27" s="1">
         <v>1569.20715</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -1802,8 +1885,11 @@
       <c r="O28" s="1">
         <v>1820.3380999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -1850,8 +1936,11 @@
       <c r="O29" s="1">
         <v>2181.5538500000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -1898,50 +1987,53 @@
       <c r="O30" s="1">
         <v>2455</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="P30" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="N32" s="21"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="20"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="20"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="20"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="20"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="20"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="20"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="2"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="22"/>
     </row>
-    <row r="67" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F67" s="23"/>
       <c r="G67" s="23"/>
       <c r="H67" s="23"/>
       <c r="I67" s="23"/>
     </row>
-    <row r="68" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E68" s="24"/>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
@@ -1950,7 +2042,7 @@
       <c r="K68" s="16"/>
       <c r="L68" s="16"/>
     </row>
-    <row r="69" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
@@ -1959,7 +2051,7 @@
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
     </row>
-    <row r="70" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
@@ -1968,7 +2060,7 @@
       <c r="K70" s="10"/>
       <c r="L70" s="10"/>
     </row>
-    <row r="71" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
@@ -1977,7 +2069,7 @@
       <c r="K71" s="10"/>
       <c r="L71" s="10"/>
     </row>
-    <row r="72" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
       <c r="H72" s="6"/>
@@ -1986,7 +2078,7 @@
       <c r="K72" s="10"/>
       <c r="L72" s="10"/>
     </row>
-    <row r="73" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
@@ -1995,7 +2087,7 @@
       <c r="K73" s="10"/>
       <c r="L73" s="10"/>
     </row>
-    <row r="74" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
       <c r="H74" s="6"/>
@@ -2004,7 +2096,7 @@
       <c r="K74" s="10"/>
       <c r="L74" s="10"/>
     </row>
-    <row r="75" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
       <c r="H75" s="6"/>
@@ -2013,7 +2105,7 @@
       <c r="K75" s="10"/>
       <c r="L75" s="10"/>
     </row>
-    <row r="76" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
@@ -2022,7 +2114,7 @@
       <c r="K76" s="10"/>
       <c r="L76" s="10"/>
     </row>
-    <row r="77" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
@@ -2031,7 +2123,7 @@
       <c r="K77" s="10"/>
       <c r="L77" s="10"/>
     </row>
-    <row r="78" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
@@ -2040,7 +2132,7 @@
       <c r="K78" s="10"/>
       <c r="L78" s="10"/>
     </row>
-    <row r="79" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
@@ -2049,7 +2141,7 @@
       <c r="K79" s="10"/>
       <c r="L79" s="10"/>
     </row>
-    <row r="80" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
@@ -2058,7 +2150,7 @@
       <c r="K80" s="10"/>
       <c r="L80" s="10"/>
     </row>
-    <row r="81" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
@@ -2067,7 +2159,7 @@
       <c r="K81" s="10"/>
       <c r="L81" s="10"/>
     </row>
-    <row r="82" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F82" s="18"/>
       <c r="G82" s="18"/>
       <c r="H82" s="6"/>
@@ -2076,7 +2168,7 @@
       <c r="K82" s="10"/>
       <c r="L82" s="10"/>
     </row>
-    <row r="83" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
       <c r="H83" s="6"/>
@@ -2085,7 +2177,7 @@
       <c r="K83" s="10"/>
       <c r="L83" s="10"/>
     </row>
-    <row r="84" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
       <c r="H84" s="6"/>
@@ -2094,7 +2186,7 @@
       <c r="K84" s="10"/>
       <c r="L84" s="10"/>
     </row>
-    <row r="85" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
@@ -2103,7 +2195,7 @@
       <c r="K85" s="10"/>
       <c r="L85" s="10"/>
     </row>
-    <row r="86" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
       <c r="H86" s="6"/>
@@ -2112,7 +2204,7 @@
       <c r="K86" s="10"/>
       <c r="L86" s="10"/>
     </row>
-    <row r="87" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
       <c r="H87" s="6"/>
@@ -2121,7 +2213,7 @@
       <c r="K87" s="10"/>
       <c r="L87" s="10"/>
     </row>
-    <row r="88" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
@@ -2130,7 +2222,7 @@
       <c r="K88" s="10"/>
       <c r="L88" s="10"/>
     </row>
-    <row r="89" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
@@ -2139,23 +2231,23 @@
       <c r="K89" s="10"/>
       <c r="L89" s="10"/>
     </row>
-    <row r="90" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J90" s="10"/>
     </row>
-    <row r="91" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F91" s="23"/>
       <c r="G91" s="23"/>
       <c r="H91" s="23"/>
       <c r="I91" s="23"/>
     </row>
-    <row r="92" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E92" s="24"/>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
     </row>
-    <row r="93" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E93" s="20"/>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
@@ -2165,7 +2257,7 @@
       <c r="K93" s="10"/>
       <c r="L93" s="10"/>
     </row>
-    <row r="94" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E94" s="20"/>
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
@@ -2175,7 +2267,7 @@
       <c r="K94" s="10"/>
       <c r="L94" s="10"/>
     </row>
-    <row r="95" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E95" s="20"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
@@ -2185,7 +2277,7 @@
       <c r="K95" s="10"/>
       <c r="L95" s="10"/>
     </row>
-    <row r="96" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E96" s="20"/>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
@@ -2195,7 +2287,7 @@
       <c r="K96" s="10"/>
       <c r="L96" s="10"/>
     </row>
-    <row r="97" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E97" s="20"/>
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
@@ -2205,7 +2297,7 @@
       <c r="K97" s="10"/>
       <c r="L97" s="10"/>
     </row>
-    <row r="98" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E98" s="20"/>
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
@@ -2215,7 +2307,7 @@
       <c r="K98" s="10"/>
       <c r="L98" s="10"/>
     </row>
-    <row r="99" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E99" s="2"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
@@ -2225,7 +2317,7 @@
       <c r="K99" s="10"/>
       <c r="L99" s="10"/>
     </row>
-    <row r="100" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E100" s="2"/>
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
@@ -2235,7 +2327,7 @@
       <c r="K100" s="10"/>
       <c r="L100" s="10"/>
     </row>
-    <row r="101" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E101" s="2"/>
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
@@ -2245,7 +2337,7 @@
       <c r="K101" s="10"/>
       <c r="L101" s="10"/>
     </row>
-    <row r="102" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E102" s="2"/>
       <c r="J102" s="10"/>
       <c r="K102" s="10"/>

</xml_diff>

<commit_message>
Ph half checkted, correct sample weights
</commit_message>
<xml_diff>
--- a/Metadaten_all_86_cleanandneat.xlsx
+++ b/Metadaten_all_86_cleanandneat.xlsx
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -535,12 +535,13 @@
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="26.3984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.296875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3984375" style="1" customWidth="1"/>
-    <col min="11" max="13" width="9" style="1"/>
-    <col min="14" max="14" width="15.5" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="12.09765625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="9" width="9" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3984375" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="13" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -633,7 +634,7 @@
         <v>2340</v>
       </c>
       <c r="P2" s="1">
-        <v>20</v>
+        <v>11.82</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -676,7 +677,7 @@
         <v>2564.2718446601939</v>
       </c>
       <c r="P3" s="1">
-        <v>20</v>
+        <v>7.26</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -719,7 +720,7 @@
         <v>3777.8640776699026</v>
       </c>
       <c r="P4" s="1">
-        <v>20</v>
+        <v>10.02</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -762,7 +763,7 @@
         <v>8729.3203883495153</v>
       </c>
       <c r="P5" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -813,7 +814,7 @@
         <v>16630</v>
       </c>
       <c r="P6" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -864,7 +865,7 @@
         <v>16544.85436893204</v>
       </c>
       <c r="P7" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -915,7 +916,7 @@
         <v>22056.369785794814</v>
       </c>
       <c r="P8" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -962,7 +963,7 @@
         <v>23420.518602029311</v>
       </c>
       <c r="P9" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1013,7 +1014,7 @@
         <v>26813.979706877115</v>
       </c>
       <c r="P10" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1064,7 +1065,7 @@
         <v>29091.319052987601</v>
       </c>
       <c r="P11" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1115,7 +1116,7 @@
         <v>34333.7091319053</v>
       </c>
       <c r="P12" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1160,7 +1161,7 @@
         <v>36239.007891770008</v>
       </c>
       <c r="P13" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1205,7 +1206,7 @@
         <v>40000</v>
       </c>
       <c r="P14" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1250,7 +1251,7 @@
         <v>41639.233370913193</v>
       </c>
       <c r="P15" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -1301,7 +1302,7 @@
         <v>38000</v>
       </c>
       <c r="P16" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -1353,7 +1354,7 @@
         <v>38900.315000000002</v>
       </c>
       <c r="P17" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -1404,7 +1405,7 @@
         <v>16915.631067961163</v>
       </c>
       <c r="P18" s="1">
-        <v>20</v>
+        <v>13.06</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -1455,7 +1456,7 @@
         <v>21770</v>
       </c>
       <c r="P19" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -1506,7 +1507,7 @@
         <v>19342.815533980582</v>
       </c>
       <c r="P20" s="1">
-        <v>20</v>
+        <v>12.22</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -1557,7 +1558,7 @@
         <v>14488.446601941747</v>
       </c>
       <c r="P21" s="1">
-        <v>20</v>
+        <v>13.81</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1601,7 +1602,7 @@
         <v>45.220700000000022</v>
       </c>
       <c r="P22" s="1">
-        <v>20</v>
+        <v>17.77</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1645,7 +1646,7 @@
         <v>175</v>
       </c>
       <c r="P23" s="1">
-        <v>20</v>
+        <v>14.226000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -1689,7 +1690,7 @@
         <v>578.44395000000009</v>
       </c>
       <c r="P24" s="1">
-        <v>20</v>
+        <v>7.44</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -1733,7 +1734,7 @@
         <v>956.86045000000013</v>
       </c>
       <c r="P25" s="1">
-        <v>20</v>
+        <v>9.9600000000000009</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1784,7 +1785,7 @@
         <v>1080</v>
       </c>
       <c r="P26" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1835,7 +1836,7 @@
         <v>1569.20715</v>
       </c>
       <c r="P27" s="1">
-        <v>20</v>
+        <v>9.67</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -1886,7 +1887,7 @@
         <v>1820.3380999999999</v>
       </c>
       <c r="P28" s="1">
-        <v>20</v>
+        <v>8.66</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -1937,7 +1938,7 @@
         <v>2181.5538500000002</v>
       </c>
       <c r="P29" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -1988,7 +1989,7 @@
         <v>2455</v>
       </c>
       <c r="P30" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fe3 nach josephine, einheiten geprüft, HCO3 Gibbs formation energy
</commit_message>
<xml_diff>
--- a/Metadaten_all_86_cleanandneat.xlsx
+++ b/Metadaten_all_86_cleanandneat.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="19">
   <si>
     <t>depth</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>weight</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P102"/>
+  <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -544,7 +547,7 @@
     <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -593,8 +596,11 @@
       <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -636,8 +642,11 @@
       <c r="P2" s="1">
         <v>11.82</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -679,8 +688,11 @@
       <c r="P3" s="1">
         <v>7.26</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -722,8 +734,11 @@
       <c r="P4" s="1">
         <v>10.02</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="1">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -765,8 +780,11 @@
       <c r="P5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -816,8 +834,11 @@
       <c r="P6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -867,8 +888,11 @@
       <c r="P7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -918,8 +942,11 @@
       <c r="P8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -965,8 +992,11 @@
       <c r="P9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1016,8 +1046,11 @@
       <c r="P10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1067,8 +1100,11 @@
       <c r="P11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1118,8 +1154,11 @@
       <c r="P12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1163,8 +1202,11 @@
       <c r="P13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1208,8 +1250,11 @@
       <c r="P14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1253,8 +1298,11 @@
       <c r="P15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1304,8 +1352,11 @@
       <c r="P16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1356,8 +1407,11 @@
       <c r="P17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1407,8 +1461,11 @@
       <c r="P18" s="1">
         <v>13.06</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q18" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1458,8 +1515,11 @@
       <c r="P19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -1509,8 +1569,11 @@
       <c r="P20" s="1">
         <v>12.22</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1560,8 +1623,11 @@
       <c r="P21" s="1">
         <v>13.81</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="1">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1604,8 +1670,11 @@
       <c r="P22" s="1">
         <v>17.77</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1648,8 +1717,11 @@
       <c r="P23" s="1">
         <v>14.226000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23" s="1">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1692,8 +1764,11 @@
       <c r="P24" s="1">
         <v>7.44</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -1736,8 +1811,11 @@
       <c r="P25" s="1">
         <v>9.9600000000000009</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="1">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1787,8 +1865,11 @@
       <c r="P26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1838,8 +1919,11 @@
       <c r="P27" s="1">
         <v>9.67</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" s="1">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -1889,8 +1973,11 @@
       <c r="P28" s="1">
         <v>8.66</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -1940,8 +2027,11 @@
       <c r="P29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -1991,8 +2081,11 @@
       <c r="P30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="N32" s="21"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>